<commit_message>
update momo, fix bugs
</commit_message>
<xml_diff>
--- a/momo/momo 訂單-冷凍.xlsx
+++ b/momo/momo 訂單-冷凍.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
   <si>
     <t>轉入頂新</t>
   </si>
@@ -93,9 +93,6 @@
     <t>30170119781263</t>
   </si>
   <si>
-    <t>3017011978</t>
-  </si>
-  <si>
     <t>鍾慧盈</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>30170121792557</t>
   </si>
   <si>
-    <t>3017012179</t>
-  </si>
-  <si>
     <t>黃芊綾</t>
   </si>
   <si>
@@ -228,9 +222,6 @@
     <t>30170123818060</t>
   </si>
   <si>
-    <t>3017012381</t>
-  </si>
-  <si>
     <t>曾惠玲</t>
   </si>
   <si>
@@ -273,9 +264,6 @@
     <t>30170124820409</t>
   </si>
   <si>
-    <t>3017012482</t>
-  </si>
-  <si>
     <t>郭玉芳</t>
   </si>
   <si>
@@ -355,9 +343,6 @@
   </si>
   <si>
     <t>30170120785279</t>
-  </si>
-  <si>
-    <t>3017012078</t>
   </si>
   <si>
     <t>陳俊瑋</t>
@@ -772,9 +757,9 @@
     <col customWidth="1" max="19" min="19" width="32"/>
     <col customWidth="1" max="20" min="20" width="8"/>
     <col customWidth="1" max="21" min="21" width="8"/>
-    <col customWidth="1" max="22" min="22" width="10"/>
-    <col customWidth="1" max="23" min="23" width="10"/>
-    <col customWidth="1" max="24" min="24" width="6"/>
+    <col customWidth="1" max="25" min="25" width="10"/>
+    <col customWidth="1" max="26" min="26" width="10"/>
+    <col customWidth="1" max="27" min="27" width="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29"/>
@@ -839,13 +824,16 @@
       <c r="U3" t="s">
         <v>18</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" t="s"/>
+      <c r="W3" t="s"/>
+      <c r="X3" t="s"/>
+      <c r="Y3" t="s">
         <v>19</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>20</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -863,52 +851,52 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J5" s="1" t="s"/>
       <c r="K5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="1" t="n"/>
       <c r="M5" s="1" t="n"/>
       <c r="N5" s="1" t="n"/>
       <c r="O5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P5" s="1" t="n"/>
       <c r="Q5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="n"/>
+      <c r="W5" s="1" t="n"/>
+      <c r="X5" s="1" t="n"/>
+      <c r="Y5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X5" s="1" t="n"/>
-      <c r="Y5" s="1" t="n"/>
-      <c r="Z5" s="1" t="n"/>
+      <c r="Z5" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA5" s="1" t="n"/>
       <c r="AB5" s="1" t="n"/>
       <c r="AC5" s="1" t="n"/>
@@ -924,639 +912,639 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s"/>
       <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s">
         <v>28</v>
-      </c>
-      <c r="O6" t="s">
-        <v>29</v>
       </c>
       <c r="Q6" t="s">
         <v>23</v>
       </c>
       <c r="R6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" t="s">
         <v>30</v>
       </c>
-      <c r="S6" t="s">
-        <v>31</v>
-      </c>
       <c r="T6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y6" t="s">
         <v>33</v>
       </c>
-      <c r="V6" t="s">
-        <v>34</v>
-      </c>
-      <c r="W6" t="s">
-        <v>35</v>
+      <c r="Z6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D7" s="1" t="n"/>
       <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="J7" s="1" t="s"/>
       <c r="K7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L7" s="1" t="n"/>
       <c r="M7" s="1" t="n"/>
       <c r="N7" s="1" t="n"/>
       <c r="O7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P7" s="1" t="n"/>
       <c r="Q7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="V7" s="1" t="n"/>
+      <c r="W7" s="1" t="n"/>
       <c r="X7" s="1" t="n"/>
-      <c r="Y7" s="1" t="n"/>
-      <c r="Z7" s="1" t="n"/>
+      <c r="Y7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA7" s="1" t="n"/>
       <c r="AB7" s="1" t="n"/>
       <c r="AC7" s="1" t="n"/>
     </row>
     <row r="8" spans="1:29">
       <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
         <v>40</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
         <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" t="s">
-        <v>43</v>
       </c>
       <c r="J8" t="s"/>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" t="s">
-        <v>39</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>45</v>
       </c>
-      <c r="S8" t="s">
+      <c r="U8" t="s">
         <v>46</v>
       </c>
-      <c r="T8" t="s">
-        <v>47</v>
-      </c>
-      <c r="U8" t="s">
-        <v>48</v>
-      </c>
-      <c r="V8" t="s">
-        <v>34</v>
-      </c>
-      <c r="W8" t="s">
-        <v>35</v>
+      <c r="Y8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:29">
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
         <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" t="s">
-        <v>43</v>
       </c>
       <c r="J9" t="s"/>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" t="s">
         <v>44</v>
       </c>
-      <c r="Q9" t="s">
-        <v>39</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>45</v>
       </c>
-      <c r="S9" t="s">
+      <c r="U9" t="s">
         <v>46</v>
       </c>
-      <c r="T9" t="s">
-        <v>47</v>
-      </c>
-      <c r="U9" t="s">
-        <v>48</v>
-      </c>
-      <c r="V9" t="s">
-        <v>34</v>
-      </c>
-      <c r="W9" t="s">
-        <v>35</v>
+      <c r="Y9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
         <v>40</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
         <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" t="s">
-        <v>43</v>
       </c>
       <c r="J10" t="s"/>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" t="s">
         <v>44</v>
       </c>
-      <c r="Q10" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>45</v>
       </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
         <v>46</v>
       </c>
-      <c r="T10" t="s">
-        <v>47</v>
-      </c>
-      <c r="U10" t="s">
-        <v>48</v>
-      </c>
-      <c r="V10" t="s">
-        <v>34</v>
-      </c>
-      <c r="W10" t="s">
-        <v>35</v>
+      <c r="Y10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:29">
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>39</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
         <v>41</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" t="s">
-        <v>43</v>
       </c>
       <c r="J11" t="s"/>
       <c r="K11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" t="s">
-        <v>39</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>45</v>
       </c>
-      <c r="S11" t="s">
+      <c r="U11" t="s">
         <v>46</v>
       </c>
-      <c r="T11" t="s">
-        <v>47</v>
-      </c>
-      <c r="U11" t="s">
-        <v>48</v>
-      </c>
-      <c r="V11" t="s">
-        <v>34</v>
-      </c>
-      <c r="W11" t="s">
-        <v>35</v>
+      <c r="Y11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>39</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="s">
         <v>41</v>
-      </c>
-      <c r="G12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" t="s">
-        <v>43</v>
       </c>
       <c r="J12" t="s"/>
       <c r="K12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>38</v>
+      </c>
+      <c r="R12" t="s">
+        <v>43</v>
+      </c>
+      <c r="S12" t="s">
         <v>44</v>
       </c>
-      <c r="Q12" t="s">
-        <v>39</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>45</v>
       </c>
-      <c r="S12" t="s">
+      <c r="U12" t="s">
         <v>46</v>
       </c>
-      <c r="T12" t="s">
-        <v>47</v>
-      </c>
-      <c r="U12" t="s">
-        <v>48</v>
-      </c>
-      <c r="V12" t="s">
-        <v>34</v>
-      </c>
-      <c r="W12" t="s">
-        <v>35</v>
+      <c r="Y12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:29">
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
         <v>40</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" t="s">
         <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" t="s">
-        <v>43</v>
       </c>
       <c r="J13" t="s"/>
       <c r="K13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" t="s">
         <v>44</v>
       </c>
-      <c r="Q13" t="s">
-        <v>39</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>45</v>
       </c>
-      <c r="S13" t="s">
+      <c r="U13" t="s">
         <v>46</v>
       </c>
-      <c r="T13" t="s">
-        <v>47</v>
-      </c>
-      <c r="U13" t="s">
-        <v>48</v>
-      </c>
-      <c r="V13" t="s">
-        <v>34</v>
-      </c>
-      <c r="W13" t="s">
-        <v>35</v>
+      <c r="Y13" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1" t="n"/>
       <c r="E14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J14" s="1" t="s"/>
       <c r="K14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L14" s="1" t="n"/>
       <c r="M14" s="1" t="n"/>
       <c r="N14" s="1" t="n"/>
       <c r="O14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P14" s="1" t="n"/>
       <c r="Q14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="T14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="V14" s="1" t="n"/>
+      <c r="W14" s="1" t="n"/>
       <c r="X14" s="1" t="n"/>
-      <c r="Y14" s="1" t="n"/>
-      <c r="Z14" s="1" t="n"/>
+      <c r="Y14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA14" s="1" t="n"/>
       <c r="AB14" s="1" t="n"/>
       <c r="AC14" s="1" t="n"/>
     </row>
     <row r="15" spans="1:29">
       <c r="B15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
         <v>49</v>
       </c>
-      <c r="E15" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" t="s">
-        <v>51</v>
-      </c>
       <c r="H15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J15" t="s"/>
       <c r="K15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S15" t="s">
+        <v>51</v>
+      </c>
+      <c r="T15" t="s">
+        <v>55</v>
+      </c>
+      <c r="U15" t="s">
         <v>53</v>
       </c>
-      <c r="T15" t="s">
-        <v>57</v>
-      </c>
-      <c r="U15" t="s">
-        <v>55</v>
-      </c>
-      <c r="V15" t="s">
-        <v>34</v>
-      </c>
-      <c r="W15" t="s">
-        <v>35</v>
+      <c r="Y15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:29">
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
         <v>49</v>
       </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" t="s">
-        <v>51</v>
-      </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J16" t="s"/>
       <c r="K16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S16" t="s">
+        <v>51</v>
+      </c>
+      <c r="T16" t="s">
+        <v>57</v>
+      </c>
+      <c r="U16" t="s">
         <v>53</v>
       </c>
-      <c r="T16" t="s">
-        <v>59</v>
-      </c>
-      <c r="U16" t="s">
-        <v>55</v>
-      </c>
-      <c r="V16" t="s">
-        <v>34</v>
-      </c>
-      <c r="W16" t="s">
-        <v>35</v>
+      <c r="Y16" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1" t="n"/>
       <c r="E17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="J17" s="1" t="s"/>
       <c r="K17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L17" s="1" t="n"/>
       <c r="M17" s="1" t="n"/>
       <c r="N17" s="1" t="n"/>
       <c r="O17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P17" s="1" t="n"/>
       <c r="Q17" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="T17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="S17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="U17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="V17" s="1" t="n"/>
+      <c r="W17" s="1" t="n"/>
       <c r="X17" s="1" t="n"/>
-      <c r="Y17" s="1" t="n"/>
-      <c r="Z17" s="1" t="n"/>
+      <c r="Y17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA17" s="1" t="n"/>
       <c r="AB17" s="1" t="n"/>
       <c r="AC17" s="1" t="n"/>
@@ -1564,749 +1552,749 @@
     <row r="18" spans="1:29">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D18" s="1" t="n"/>
       <c r="E18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J18" s="1" t="s"/>
       <c r="K18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L18" s="1" t="n"/>
       <c r="M18" s="1" t="n"/>
       <c r="N18" s="1" t="n"/>
       <c r="O18" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P18" s="1" t="n"/>
       <c r="Q18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="V18" s="1" t="n"/>
+      <c r="W18" s="1" t="n"/>
       <c r="X18" s="1" t="n"/>
-      <c r="Y18" s="1" t="n"/>
-      <c r="Z18" s="1" t="n"/>
+      <c r="Y18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA18" s="1" t="n"/>
       <c r="AB18" s="1" t="n"/>
       <c r="AC18" s="1" t="n"/>
     </row>
     <row r="19" spans="1:29">
       <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
         <v>67</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
         <v>68</v>
       </c>
-      <c r="E19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" t="s">
-        <v>71</v>
-      </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J19" t="s"/>
       <c r="K19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O19" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>66</v>
+      </c>
+      <c r="R19" t="s">
+        <v>70</v>
+      </c>
+      <c r="S19" t="s">
+        <v>71</v>
+      </c>
+      <c r="T19" t="s">
+        <v>74</v>
+      </c>
+      <c r="U19" t="s">
         <v>72</v>
       </c>
-      <c r="Q19" t="s">
-        <v>68</v>
-      </c>
-      <c r="R19" t="s">
-        <v>73</v>
-      </c>
-      <c r="S19" t="s">
-        <v>74</v>
-      </c>
-      <c r="T19" t="s">
-        <v>77</v>
-      </c>
-      <c r="U19" t="s">
-        <v>75</v>
-      </c>
-      <c r="V19" t="s">
-        <v>34</v>
-      </c>
-      <c r="W19" t="s">
-        <v>35</v>
+      <c r="Y19" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:29">
       <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
         <v>67</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" t="s">
         <v>68</v>
       </c>
-      <c r="E20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" t="s">
-        <v>71</v>
-      </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J20" t="s"/>
       <c r="K20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O20" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>66</v>
+      </c>
+      <c r="R20" t="s">
+        <v>70</v>
+      </c>
+      <c r="S20" t="s">
+        <v>71</v>
+      </c>
+      <c r="T20" t="s">
+        <v>74</v>
+      </c>
+      <c r="U20" t="s">
         <v>72</v>
       </c>
-      <c r="Q20" t="s">
-        <v>68</v>
-      </c>
-      <c r="R20" t="s">
-        <v>73</v>
-      </c>
-      <c r="S20" t="s">
-        <v>74</v>
-      </c>
-      <c r="T20" t="s">
-        <v>77</v>
-      </c>
-      <c r="U20" t="s">
-        <v>75</v>
-      </c>
-      <c r="V20" t="s">
-        <v>34</v>
-      </c>
-      <c r="W20" t="s">
-        <v>35</v>
+      <c r="Y20" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:29">
       <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
         <v>67</v>
       </c>
-      <c r="C21" t="s">
+      <c r="F21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" t="s">
         <v>68</v>
       </c>
-      <c r="E21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" t="s">
-        <v>71</v>
-      </c>
       <c r="H21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J21" t="s"/>
       <c r="K21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O21" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>66</v>
+      </c>
+      <c r="R21" t="s">
+        <v>70</v>
+      </c>
+      <c r="S21" t="s">
+        <v>71</v>
+      </c>
+      <c r="T21" t="s">
+        <v>76</v>
+      </c>
+      <c r="U21" t="s">
         <v>72</v>
       </c>
-      <c r="Q21" t="s">
-        <v>68</v>
-      </c>
-      <c r="R21" t="s">
-        <v>73</v>
-      </c>
-      <c r="S21" t="s">
-        <v>74</v>
-      </c>
-      <c r="T21" t="s">
-        <v>79</v>
-      </c>
-      <c r="U21" t="s">
-        <v>75</v>
-      </c>
-      <c r="V21" t="s">
-        <v>34</v>
-      </c>
-      <c r="W21" t="s">
-        <v>35</v>
+      <c r="Y21" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:29">
       <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
+      <c r="F22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" t="s">
         <v>68</v>
       </c>
-      <c r="E22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" t="s">
-        <v>71</v>
-      </c>
       <c r="H22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J22" t="s"/>
       <c r="K22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O22" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>66</v>
+      </c>
+      <c r="R22" t="s">
+        <v>70</v>
+      </c>
+      <c r="S22" t="s">
+        <v>71</v>
+      </c>
+      <c r="T22" t="s">
+        <v>78</v>
+      </c>
+      <c r="U22" t="s">
         <v>72</v>
       </c>
-      <c r="Q22" t="s">
-        <v>68</v>
-      </c>
-      <c r="R22" t="s">
-        <v>73</v>
-      </c>
-      <c r="S22" t="s">
-        <v>74</v>
-      </c>
-      <c r="T22" t="s">
-        <v>81</v>
-      </c>
-      <c r="U22" t="s">
-        <v>75</v>
-      </c>
-      <c r="V22" t="s">
-        <v>34</v>
-      </c>
-      <c r="W22" t="s">
-        <v>35</v>
+      <c r="Y22" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:29">
       <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
         <v>67</v>
       </c>
-      <c r="C23" t="s">
+      <c r="F23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" t="s">
         <v>68</v>
       </c>
-      <c r="E23" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" t="s">
-        <v>71</v>
-      </c>
       <c r="H23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J23" t="s"/>
       <c r="K23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O23" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>66</v>
+      </c>
+      <c r="R23" t="s">
+        <v>70</v>
+      </c>
+      <c r="S23" t="s">
+        <v>71</v>
+      </c>
+      <c r="T23" t="s">
+        <v>36</v>
+      </c>
+      <c r="U23" t="s">
         <v>72</v>
       </c>
-      <c r="Q23" t="s">
-        <v>68</v>
-      </c>
-      <c r="R23" t="s">
-        <v>73</v>
-      </c>
-      <c r="S23" t="s">
-        <v>74</v>
-      </c>
-      <c r="T23" t="s">
-        <v>37</v>
-      </c>
-      <c r="U23" t="s">
-        <v>75</v>
-      </c>
-      <c r="V23" t="s">
-        <v>34</v>
-      </c>
-      <c r="W23" t="s">
-        <v>35</v>
+      <c r="Y23" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:29">
       <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="F24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" t="s">
         <v>68</v>
       </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" t="s">
-        <v>71</v>
-      </c>
       <c r="H24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J24" t="s"/>
       <c r="K24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O24" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>66</v>
+      </c>
+      <c r="R24" t="s">
+        <v>70</v>
+      </c>
+      <c r="S24" t="s">
+        <v>71</v>
+      </c>
+      <c r="T24" t="s">
+        <v>36</v>
+      </c>
+      <c r="U24" t="s">
         <v>72</v>
       </c>
-      <c r="Q24" t="s">
-        <v>68</v>
-      </c>
-      <c r="R24" t="s">
-        <v>73</v>
-      </c>
-      <c r="S24" t="s">
-        <v>74</v>
-      </c>
-      <c r="T24" t="s">
-        <v>37</v>
-      </c>
-      <c r="U24" t="s">
-        <v>75</v>
-      </c>
-      <c r="V24" t="s">
-        <v>34</v>
-      </c>
-      <c r="W24" t="s">
-        <v>35</v>
+      <c r="Y24" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:29">
       <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" t="s">
         <v>67</v>
       </c>
-      <c r="C25" t="s">
+      <c r="F25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" t="s">
         <v>68</v>
       </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" t="s">
-        <v>71</v>
-      </c>
       <c r="H25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J25" t="s"/>
       <c r="K25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O25" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R25" t="s">
+        <v>70</v>
+      </c>
+      <c r="S25" t="s">
+        <v>71</v>
+      </c>
+      <c r="T25" t="s">
+        <v>78</v>
+      </c>
+      <c r="U25" t="s">
         <v>72</v>
       </c>
-      <c r="Q25" t="s">
-        <v>68</v>
-      </c>
-      <c r="R25" t="s">
-        <v>73</v>
-      </c>
-      <c r="S25" t="s">
-        <v>74</v>
-      </c>
-      <c r="T25" t="s">
-        <v>81</v>
-      </c>
-      <c r="U25" t="s">
-        <v>75</v>
-      </c>
-      <c r="V25" t="s">
-        <v>34</v>
-      </c>
-      <c r="W25" t="s">
-        <v>35</v>
+      <c r="Y25" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D26" s="1" t="n"/>
       <c r="E26" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J26" s="1" t="s"/>
       <c r="K26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L26" s="1" t="n"/>
       <c r="M26" s="1" t="n"/>
       <c r="N26" s="1" t="n"/>
       <c r="O26" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P26" s="1" t="n"/>
       <c r="Q26" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="V26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="V26" s="1" t="n"/>
+      <c r="W26" s="1" t="n"/>
       <c r="X26" s="1" t="n"/>
-      <c r="Y26" s="1" t="n"/>
-      <c r="Z26" s="1" t="n"/>
+      <c r="Y26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA26" s="1" t="n"/>
       <c r="AB26" s="1" t="n"/>
       <c r="AC26" s="1" t="n"/>
     </row>
     <row r="27" spans="1:29">
       <c r="B27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J27" t="s"/>
       <c r="K27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="T27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U27" t="s">
-        <v>91</v>
-      </c>
-      <c r="V27" t="s">
-        <v>34</v>
-      </c>
-      <c r="W27" t="s">
-        <v>35</v>
+        <v>87</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:29">
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I28" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J28" t="s"/>
       <c r="K28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S28" t="s">
+        <v>85</v>
+      </c>
+      <c r="T28" t="s">
         <v>89</v>
       </c>
-      <c r="T28" t="s">
-        <v>93</v>
-      </c>
       <c r="U28" t="s">
-        <v>91</v>
-      </c>
-      <c r="V28" t="s">
-        <v>34</v>
-      </c>
-      <c r="W28" t="s">
-        <v>35</v>
+        <v>87</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:29">
       <c r="B29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J29" t="s"/>
       <c r="K29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S29" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="T29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="U29" t="s">
-        <v>91</v>
-      </c>
-      <c r="V29" t="s">
-        <v>34</v>
-      </c>
-      <c r="W29" t="s">
-        <v>35</v>
+        <v>87</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:29">
       <c r="B30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J30" t="s"/>
       <c r="K30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="T30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U30" t="s">
-        <v>91</v>
-      </c>
-      <c r="V30" t="s">
-        <v>34</v>
-      </c>
-      <c r="W30" t="s">
-        <v>35</v>
+        <v>87</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D31" s="1" t="n"/>
       <c r="E31" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J31" s="1" t="s"/>
       <c r="K31" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L31" s="1" t="n"/>
       <c r="M31" s="1" t="n"/>
       <c r="N31" s="1" t="n"/>
       <c r="O31" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P31" s="1" t="n"/>
       <c r="Q31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="S31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="R31" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="T31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W31" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="V31" s="1" t="n"/>
+      <c r="W31" s="1" t="n"/>
       <c r="X31" s="1" t="n"/>
-      <c r="Y31" s="1" t="n"/>
-      <c r="Z31" s="1" t="n"/>
+      <c r="Y31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA31" s="1" t="n"/>
       <c r="AB31" s="1" t="n"/>
       <c r="AC31" s="1" t="n"/>
@@ -2314,319 +2302,319 @@
     <row r="32" spans="1:29">
       <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D32" s="1" t="n"/>
       <c r="E32" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J32" s="1" t="s"/>
       <c r="K32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L32" s="1" t="n"/>
       <c r="M32" s="1" t="n"/>
       <c r="N32" s="1" t="n"/>
       <c r="O32" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P32" s="1" t="n"/>
       <c r="Q32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="R32" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="S32" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="T32" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W32" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="V32" s="1" t="n"/>
+      <c r="W32" s="1" t="n"/>
       <c r="X32" s="1" t="n"/>
-      <c r="Y32" s="1" t="n"/>
-      <c r="Z32" s="1" t="n"/>
+      <c r="Y32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA32" s="1" t="n"/>
       <c r="AB32" s="1" t="n"/>
       <c r="AC32" s="1" t="n"/>
     </row>
     <row r="33" spans="1:29">
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F33" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J33" t="s"/>
       <c r="K33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q33" t="s">
+        <v>96</v>
+      </c>
+      <c r="R33" t="s">
         <v>100</v>
       </c>
-      <c r="R33" t="s">
-        <v>104</v>
-      </c>
       <c r="S33" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="T33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="U33" t="s">
-        <v>107</v>
-      </c>
-      <c r="V33" t="s">
-        <v>34</v>
-      </c>
-      <c r="W33" t="s">
-        <v>35</v>
+        <v>103</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:29">
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G34" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H34" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I34" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J34" t="s"/>
       <c r="K34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q34" t="s">
+        <v>96</v>
+      </c>
+      <c r="R34" t="s">
         <v>100</v>
       </c>
-      <c r="R34" t="s">
-        <v>104</v>
-      </c>
       <c r="S34" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="T34" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="U34" t="s">
-        <v>107</v>
-      </c>
-      <c r="V34" t="s">
-        <v>34</v>
-      </c>
-      <c r="W34" t="s">
-        <v>35</v>
+        <v>103</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:29">
       <c r="B35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I35" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J35" t="s"/>
       <c r="K35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q35" t="s">
+        <v>96</v>
+      </c>
+      <c r="R35" t="s">
         <v>100</v>
       </c>
-      <c r="R35" t="s">
-        <v>104</v>
-      </c>
       <c r="S35" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="T35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="U35" t="s">
-        <v>107</v>
-      </c>
-      <c r="V35" t="s">
-        <v>34</v>
-      </c>
-      <c r="W35" t="s">
-        <v>35</v>
+        <v>103</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:29">
       <c r="B36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F36" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G36" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H36" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J36" t="s"/>
       <c r="K36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q36" t="s">
+        <v>96</v>
+      </c>
+      <c r="R36" t="s">
         <v>100</v>
       </c>
-      <c r="R36" t="s">
-        <v>104</v>
-      </c>
       <c r="S36" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="T36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="U36" t="s">
-        <v>107</v>
-      </c>
-      <c r="V36" t="s">
-        <v>34</v>
-      </c>
-      <c r="W36" t="s">
-        <v>35</v>
+        <v>103</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:29">
       <c r="B37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F37" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G37" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H37" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I37" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J37" t="s"/>
       <c r="K37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O37" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q37" t="s">
+        <v>96</v>
+      </c>
+      <c r="R37" t="s">
         <v>100</v>
       </c>
-      <c r="R37" t="s">
-        <v>104</v>
-      </c>
       <c r="S37" t="s">
+        <v>101</v>
+      </c>
+      <c r="T37" t="s">
         <v>105</v>
       </c>
-      <c r="T37" t="s">
-        <v>109</v>
-      </c>
       <c r="U37" t="s">
-        <v>107</v>
-      </c>
-      <c r="V37" t="s">
-        <v>34</v>
-      </c>
-      <c r="W37" t="s">
-        <v>35</v>
+        <v>103</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:29"/>
@@ -2668,9 +2656,9 @@
     <col customWidth="1" max="19" min="19" width="24"/>
     <col customWidth="1" max="20" min="20" width="8"/>
     <col customWidth="1" max="21" min="21" width="8"/>
-    <col customWidth="1" max="22" min="22" width="10"/>
-    <col customWidth="1" max="23" min="23" width="10"/>
-    <col customWidth="1" max="24" min="24" width="6"/>
+    <col customWidth="1" max="25" min="25" width="10"/>
+    <col customWidth="1" max="26" min="26" width="10"/>
+    <col customWidth="1" max="27" min="27" width="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29"/>
@@ -2735,13 +2723,16 @@
       <c r="U3" t="s">
         <v>18</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" t="s"/>
+      <c r="W3" t="s"/>
+      <c r="X3" t="s"/>
+      <c r="Y3" t="s">
         <v>19</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>20</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2749,382 +2740,382 @@
     <row r="5" spans="1:29">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D5" s="1" t="n"/>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="1" t="s"/>
       <c r="K5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="1" t="n"/>
       <c r="M5" s="1" t="n"/>
       <c r="N5" s="1" t="n"/>
       <c r="O5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P5" s="1" t="n"/>
       <c r="Q5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="R5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="T5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="V5" s="1" t="n"/>
+      <c r="W5" s="1" t="n"/>
       <c r="X5" s="1" t="n"/>
-      <c r="Y5" s="1" t="n"/>
-      <c r="Z5" s="1" t="n"/>
+      <c r="Y5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA5" s="1" t="n"/>
       <c r="AB5" s="1" t="n"/>
       <c r="AC5" s="1" t="n"/>
     </row>
     <row r="6" spans="1:29">
       <c r="B6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" t="s">
         <v>114</v>
-      </c>
-      <c r="H6" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" t="s">
-        <v>119</v>
       </c>
       <c r="J6" t="s"/>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R6" t="s">
+        <v>110</v>
+      </c>
+      <c r="S6" t="s">
         <v>111</v>
       </c>
-      <c r="R6" t="s">
-        <v>115</v>
-      </c>
-      <c r="S6" t="s">
-        <v>116</v>
-      </c>
       <c r="T6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="U6" t="s">
-        <v>117</v>
-      </c>
-      <c r="V6" t="s">
-        <v>118</v>
-      </c>
-      <c r="W6" t="s">
-        <v>35</v>
+        <v>112</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:29">
       <c r="B7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" t="s">
         <v>114</v>
-      </c>
-      <c r="H7" t="s">
-        <v>114</v>
-      </c>
-      <c r="I7" t="s">
-        <v>119</v>
       </c>
       <c r="J7" t="s"/>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q7" t="s">
+        <v>107</v>
+      </c>
+      <c r="R7" t="s">
+        <v>110</v>
+      </c>
+      <c r="S7" t="s">
         <v>111</v>
       </c>
-      <c r="R7" t="s">
-        <v>115</v>
-      </c>
-      <c r="S7" t="s">
-        <v>116</v>
-      </c>
       <c r="T7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="U7" t="s">
-        <v>117</v>
-      </c>
-      <c r="V7" t="s">
-        <v>118</v>
-      </c>
-      <c r="W7" t="s">
-        <v>35</v>
+        <v>112</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D8" s="1" t="n"/>
       <c r="E8" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J8" s="1" t="s"/>
       <c r="K8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="1" t="n"/>
       <c r="M8" s="1" t="n"/>
       <c r="N8" s="1" t="n"/>
       <c r="O8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P8" s="1" t="n"/>
       <c r="Q8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="R8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="V8" s="1" t="n"/>
+      <c r="W8" s="1" t="n"/>
       <c r="X8" s="1" t="n"/>
-      <c r="Y8" s="1" t="n"/>
-      <c r="Z8" s="1" t="n"/>
+      <c r="Y8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="AA8" s="1" t="n"/>
       <c r="AB8" s="1" t="n"/>
       <c r="AC8" s="1" t="n"/>
     </row>
     <row r="9" spans="1:29">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s"/>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q9" t="s">
+        <v>115</v>
+      </c>
+      <c r="R9" t="s">
+        <v>118</v>
+      </c>
+      <c r="S9" t="s">
+        <v>119</v>
+      </c>
+      <c r="T9" t="s">
+        <v>76</v>
+      </c>
+      <c r="U9" t="s">
         <v>120</v>
       </c>
-      <c r="R9" t="s">
-        <v>123</v>
-      </c>
-      <c r="S9" t="s">
-        <v>124</v>
-      </c>
-      <c r="T9" t="s">
-        <v>79</v>
-      </c>
-      <c r="U9" t="s">
-        <v>125</v>
-      </c>
-      <c r="V9" t="s">
-        <v>118</v>
-      </c>
-      <c r="W9" t="s">
-        <v>35</v>
+      <c r="Y9" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" t="s">
         <v>121</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>122</v>
-      </c>
-      <c r="H10" t="s">
-        <v>122</v>
-      </c>
-      <c r="I10" t="s">
-        <v>126</v>
       </c>
       <c r="J10" t="s"/>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R10" t="s">
+        <v>118</v>
+      </c>
+      <c r="S10" t="s">
+        <v>119</v>
+      </c>
+      <c r="T10" t="s">
+        <v>122</v>
+      </c>
+      <c r="U10" t="s">
         <v>120</v>
       </c>
-      <c r="R10" t="s">
-        <v>123</v>
-      </c>
-      <c r="S10" t="s">
-        <v>124</v>
-      </c>
-      <c r="T10" t="s">
-        <v>127</v>
-      </c>
-      <c r="U10" t="s">
-        <v>125</v>
-      </c>
-      <c r="V10" t="s">
-        <v>118</v>
-      </c>
-      <c r="W10" t="s">
-        <v>35</v>
+      <c r="Y10" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:29">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J11" t="s"/>
       <c r="K11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q11" t="s">
+        <v>115</v>
+      </c>
+      <c r="R11" t="s">
+        <v>118</v>
+      </c>
+      <c r="S11" t="s">
+        <v>119</v>
+      </c>
+      <c r="T11" t="s">
+        <v>89</v>
+      </c>
+      <c r="U11" t="s">
         <v>120</v>
       </c>
-      <c r="R11" t="s">
-        <v>123</v>
-      </c>
-      <c r="S11" t="s">
-        <v>124</v>
-      </c>
-      <c r="T11" t="s">
-        <v>93</v>
-      </c>
-      <c r="U11" t="s">
-        <v>125</v>
-      </c>
-      <c r="V11" t="s">
-        <v>118</v>
-      </c>
-      <c r="W11" t="s">
-        <v>35</v>
+      <c r="Y11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:29"/>
@@ -3139,7 +3130,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3166,14 +3157,14 @@
     <col customWidth="1" max="19" min="19" width="8"/>
     <col customWidth="1" max="20" min="20" width="8"/>
     <col customWidth="1" max="21" min="21" width="6"/>
-    <col customWidth="1" max="22" min="22" width="10"/>
-    <col customWidth="1" max="23" min="23" width="10"/>
-    <col customWidth="1" max="24" min="24" width="6"/>
+    <col customWidth="1" max="25" min="25" width="10"/>
+    <col customWidth="1" max="26" min="26" width="10"/>
+    <col customWidth="1" max="27" min="27" width="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24"/>
-    <row r="2" spans="1:24"/>
-    <row r="3" spans="1:24">
+    <row r="1" spans="1:27"/>
+    <row r="2" spans="1:27"/>
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3233,13 +3224,16 @@
       <c r="U3" t="s">
         <v>18</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" t="s"/>
+      <c r="W3" t="s"/>
+      <c r="X3" t="s"/>
+      <c r="Y3" t="s">
         <v>19</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>20</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change momo payment method field
</commit_message>
<xml_diff>
--- a/momo/momo 訂單-冷凍.xlsx
+++ b/momo/momo 訂單-冷凍.xlsx
@@ -117,7 +117,7 @@
     <t>1128</t>
   </si>
   <si>
-    <t>信用卡</t>
+    <t>13</t>
   </si>
   <si>
     <t>已付款</t>
@@ -357,7 +357,7 @@
     <t>1397</t>
   </si>
   <si>
-    <t>ATM</t>
+    <t>12</t>
   </si>
   <si>
     <t>鮮蝦水餃 20顆/盒(400G±10)</t>

</xml_diff>